<commit_message>
DemoData, README and requirements
New DemoData, a new README file (to be completed in github itself) and a requirements text file on dependencies
</commit_message>
<xml_diff>
--- a/DemoData/Demo_with_Data.xlsx
+++ b/DemoData/Demo_with_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="106">
   <si>
     <t>PROGRAMAÇÃO SEMANAL DE URGÊNCIAS</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Demo Client 4</t>
-  </si>
-  <si>
-    <t>Obra de Livro "7 Olhares Sobre Viseu"</t>
   </si>
   <si>
     <t>Pré Impressão</t>
@@ -363,7 +360,7 @@
     <font>
       <b val="1"/>
       <sz val="28"/>
-      <color indexed="11"/>
+      <color indexed="12"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -387,13 +384,13 @@
     <font>
       <b val="1"/>
       <sz val="18"/>
-      <color indexed="11"/>
+      <color indexed="12"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b val="1"/>
       <sz val="24"/>
-      <color indexed="11"/>
+      <color indexed="12"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -415,18 +412,18 @@
     </font>
     <font>
       <sz val="18"/>
-      <color indexed="11"/>
+      <color indexed="12"/>
       <name val="Arial"/>
     </font>
     <font>
       <b val="1"/>
       <sz val="18"/>
-      <color indexed="13"/>
+      <color indexed="9"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="18"/>
-      <color indexed="13"/>
+      <color indexed="9"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -501,13 +498,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -531,7 +528,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="11"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -546,14 +543,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -561,7 +558,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="medium">
         <color indexed="8"/>
@@ -571,43 +568,43 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="medium">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -616,7 +613,7 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="medium">
         <color indexed="8"/>
@@ -628,10 +625,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="medium">
         <color indexed="8"/>
@@ -643,7 +640,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="medium">
         <color indexed="8"/>
@@ -661,19 +658,19 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="medium">
@@ -698,7 +695,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="medium">
         <color indexed="8"/>
@@ -710,13 +707,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -725,16 +722,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -758,13 +755,13 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -779,7 +776,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -788,7 +785,7 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
@@ -800,10 +797,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
@@ -815,7 +812,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
@@ -836,7 +833,7 @@
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -845,13 +842,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -861,30 +858,30 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
@@ -912,7 +909,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom/>
@@ -920,23 +917,23 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
@@ -946,25 +943,25 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom/>
@@ -972,10 +969,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="medium">
@@ -1065,16 +1062,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="medium">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1091,148 +1088,148 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="10" fillId="5" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="11" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="11" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="10" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="10" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="10" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="12" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="12" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="13" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="16" fontId="13" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="16" fontId="13" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="16" fontId="11" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="16" fontId="11" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="10" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="6" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1250,58 +1247,58 @@
     <xf numFmtId="16" fontId="13" fillId="6" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="10" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="14" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="11" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="10" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="10" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="10" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="10" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="11" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="10" fillId="5" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1310,31 +1307,31 @@
     <xf numFmtId="49" fontId="10" fillId="5" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="10" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="11" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="10" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="12" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="14" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="14" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="10" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="15" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="10" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="10" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="10" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="16" fillId="7" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1349,37 +1346,37 @@
     <xf numFmtId="3" fontId="16" fillId="7" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="19" fillId="7" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1397,79 +1394,79 @@
     <xf numFmtId="0" fontId="23" fillId="7" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="36" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="36" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="24" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="24" fillId="3" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="24" fillId="4" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="27" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="25" fillId="3" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="25" fillId="4" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="38" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="38" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="24" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="24" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="40" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="4" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="41" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" borderId="42" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="42" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="42" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="3" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1498,11 +1495,11 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffb8cce4"/>
       <rgbColor rgb="ffff0000"/>
       <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff95b3d7"/>
       <rgbColor rgb="fffabf8f"/>
       <rgbColor rgb="ffe36c09"/>
@@ -1762,12 +1759,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1799,10 +1796,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2041,12 +2038,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -2350,10 +2347,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2947,21 +2944,21 @@
         <v>24</v>
       </c>
       <c r="D10" t="s" s="41">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E10" s="42">
         <v>200</v>
       </c>
       <c r="F10" t="s" s="41">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G10" s="43"/>
       <c r="H10" t="s" s="41">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I10" s="43"/>
       <c r="J10" t="s" s="45">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K10" s="47"/>
       <c r="L10" s="30"/>
@@ -2986,21 +2983,21 @@
         <v>20241316</v>
       </c>
       <c r="C11" t="s" s="40">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s" s="41">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E11" s="42">
         <v>12</v>
       </c>
       <c r="F11" t="s" s="41">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G11" s="43"/>
       <c r="H11" s="43"/>
       <c r="I11" t="s" s="41">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J11" s="44"/>
       <c r="K11" s="48"/>
@@ -3026,21 +3023,21 @@
         <v>20241364</v>
       </c>
       <c r="C12" t="s" s="40">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s" s="41">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E12" s="42">
         <v>40</v>
       </c>
       <c r="F12" t="s" s="41">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12" s="43"/>
       <c r="H12" s="43"/>
       <c r="I12" t="s" s="41">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J12" s="44"/>
       <c r="K12" s="47"/>
@@ -3066,7 +3063,7 @@
         <v>20241349</v>
       </c>
       <c r="C13" t="s" s="40">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s" s="41">
         <v>15</v>
@@ -3106,16 +3103,16 @@
         <v>20241318</v>
       </c>
       <c r="C14" t="s" s="40">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s" s="41">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="49">
         <v>100000</v>
       </c>
       <c r="F14" t="s" s="41">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s" s="41">
         <v>17</v>
@@ -3126,7 +3123,7 @@
         <v>22</v>
       </c>
       <c r="K14" t="s" s="41">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L14" s="30"/>
       <c r="M14" s="31"/>
@@ -3150,16 +3147,16 @@
         <v>20241354</v>
       </c>
       <c r="C15" t="s" s="40">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D15" t="s" s="41">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E15" s="42">
         <v>5000</v>
       </c>
       <c r="F15" t="s" s="41">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s" s="41">
         <v>17</v>
@@ -3190,16 +3187,16 @@
         <v>20241170</v>
       </c>
       <c r="C16" t="s" s="40">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D16" t="s" s="41">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E16" s="42">
         <v>20</v>
       </c>
       <c r="F16" t="s" s="41">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G16" t="s" s="41">
         <v>17</v>
@@ -3207,7 +3204,7 @@
       <c r="H16" s="43"/>
       <c r="I16" s="43"/>
       <c r="J16" t="s" s="45">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K16" s="47"/>
       <c r="L16" s="30"/>
@@ -3232,7 +3229,7 @@
         <v>20240942</v>
       </c>
       <c r="C17" t="s" s="40">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s" s="41">
         <v>15</v>
@@ -3241,7 +3238,7 @@
         <v>150</v>
       </c>
       <c r="F17" t="s" s="41">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G17" t="s" s="41">
         <v>17</v>
@@ -3274,7 +3271,7 @@
         <v>20240980</v>
       </c>
       <c r="C18" t="s" s="40">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s" s="41">
         <v>15</v>
@@ -3283,7 +3280,7 @@
         <v>1000</v>
       </c>
       <c r="F18" t="s" s="41">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G18" t="s" s="41">
         <v>17</v>
@@ -3314,20 +3311,20 @@
         <v>20241050</v>
       </c>
       <c r="C19" t="s" s="40">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s" s="41">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="42">
         <v>500</v>
       </c>
       <c r="F19" t="s" s="41">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G19" s="43"/>
       <c r="H19" t="s" s="41">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I19" s="43"/>
       <c r="J19" t="s" s="45">
@@ -3356,10 +3353,10 @@
         <v>20240413</v>
       </c>
       <c r="C20" t="s" s="40">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" t="s" s="41">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" s="42">
         <v>100</v>
@@ -3398,16 +3395,16 @@
         <v>20240583</v>
       </c>
       <c r="C21" t="s" s="50">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s" s="51">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="52">
         <v>20000</v>
       </c>
       <c r="F21" t="s" s="51">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G21" t="s" s="51">
         <v>17</v>
@@ -3415,7 +3412,7 @@
       <c r="H21" s="53"/>
       <c r="I21" s="53"/>
       <c r="J21" t="s" s="51">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K21" s="54"/>
       <c r="L21" s="30"/>
@@ -3440,20 +3437,20 @@
         <v>20241341</v>
       </c>
       <c r="C22" t="s" s="40">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D22" t="s" s="41">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E22" s="42">
         <v>30</v>
       </c>
       <c r="F22" t="s" s="41">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G22" s="43"/>
       <c r="H22" t="s" s="41">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I22" s="43"/>
       <c r="J22" s="44"/>
@@ -3480,21 +3477,21 @@
         <v>20241305</v>
       </c>
       <c r="C23" t="s" s="40">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" t="s" s="41">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" s="42">
         <v>30</v>
       </c>
       <c r="F23" t="s" s="41">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G23" s="43"/>
       <c r="H23" s="43"/>
       <c r="I23" t="s" s="41">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J23" s="44"/>
       <c r="K23" s="48"/>
@@ -3520,24 +3517,24 @@
         <v>20241282</v>
       </c>
       <c r="C24" t="s" s="40">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s" s="41">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="42">
         <v>6000</v>
       </c>
       <c r="F24" t="s" s="41">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G24" s="43"/>
       <c r="H24" s="43"/>
       <c r="I24" t="s" s="41">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J24" t="s" s="45">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K24" s="47"/>
       <c r="L24" s="30"/>
@@ -3562,16 +3559,16 @@
         <v>20240909</v>
       </c>
       <c r="C25" t="s" s="40">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s" s="41">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E25" s="42">
         <v>2</v>
       </c>
       <c r="F25" t="s" s="41">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G25" t="s" s="41">
         <v>17</v>
@@ -3582,7 +3579,7 @@
         <v>22</v>
       </c>
       <c r="K25" t="s" s="41">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L25" s="30"/>
       <c r="M25" s="31"/>
@@ -3606,16 +3603,16 @@
         <v>20241370</v>
       </c>
       <c r="C26" t="s" s="40">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s" s="41">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E26" s="42">
         <v>3000</v>
       </c>
       <c r="F26" t="s" s="41">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G26" t="s" s="41">
         <v>17</v>
@@ -3646,21 +3643,21 @@
         <v>20241405</v>
       </c>
       <c r="C27" t="s" s="40">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s" s="41">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E27" s="42">
         <v>100</v>
       </c>
       <c r="F27" t="s" s="41">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G27" s="43"/>
       <c r="H27" s="43"/>
       <c r="I27" t="s" s="41">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J27" s="44"/>
       <c r="K27" s="47"/>
@@ -3686,21 +3683,21 @@
         <v>20241384</v>
       </c>
       <c r="C28" t="s" s="40">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D28" t="s" s="41">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E28" s="42">
         <v>1000</v>
       </c>
       <c r="F28" t="s" s="41">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G28" s="43"/>
       <c r="H28" s="43"/>
       <c r="I28" t="s" s="41">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J28" s="44"/>
       <c r="K28" s="48"/>
@@ -3726,10 +3723,10 @@
         <v>20241393</v>
       </c>
       <c r="C29" t="s" s="40">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D29" t="s" s="41">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E29" s="42">
         <v>950</v>
@@ -3766,25 +3763,25 @@
         <v>20241359</v>
       </c>
       <c r="C30" t="s" s="40">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D30" t="s" s="41">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E30" s="42">
         <v>1000</v>
       </c>
       <c r="F30" t="s" s="41">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G30" s="43"/>
       <c r="H30" s="43"/>
       <c r="I30" t="s" s="41">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J30" s="44"/>
       <c r="K30" t="s" s="56">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L30" s="30"/>
       <c r="M30" s="31"/>
@@ -3808,10 +3805,10 @@
         <v>20241389</v>
       </c>
       <c r="C31" t="s" s="40">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D31" t="s" s="41">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E31" s="42">
         <v>80</v>
@@ -3848,10 +3845,10 @@
         <v>20241404</v>
       </c>
       <c r="C32" t="s" s="40">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D32" t="s" s="41">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E32" s="42">
         <v>50</v>
@@ -3862,7 +3859,7 @@
       <c r="G32" s="43"/>
       <c r="H32" s="43"/>
       <c r="I32" t="s" s="41">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J32" s="44"/>
       <c r="K32" s="47"/>
@@ -3888,10 +3885,10 @@
         <v>20241392</v>
       </c>
       <c r="C33" t="s" s="40">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D33" t="s" s="41">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E33" s="42">
         <v>500</v>
@@ -3928,13 +3925,13 @@
         <v>20241394</v>
       </c>
       <c r="C34" t="s" s="40">
+        <v>84</v>
+      </c>
+      <c r="D34" t="s" s="41">
         <v>85</v>
       </c>
-      <c r="D34" t="s" s="41">
+      <c r="E34" t="s" s="41">
         <v>86</v>
-      </c>
-      <c r="E34" t="s" s="41">
-        <v>87</v>
       </c>
       <c r="F34" t="s" s="41">
         <v>16</v>
@@ -3968,21 +3965,21 @@
         <v>20241399</v>
       </c>
       <c r="C35" t="s" s="40">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D35" t="s" s="41">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E35" s="42">
         <v>20000</v>
       </c>
       <c r="F35" t="s" s="41">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G35" s="43"/>
       <c r="H35" s="43"/>
       <c r="I35" t="s" s="41">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J35" s="44"/>
       <c r="K35" s="47"/>
@@ -4008,16 +4005,16 @@
         <v>20241391</v>
       </c>
       <c r="C36" t="s" s="40">
+        <v>89</v>
+      </c>
+      <c r="D36" t="s" s="41">
         <v>90</v>
       </c>
-      <c r="D36" t="s" s="41">
+      <c r="E36" t="s" s="41">
         <v>91</v>
       </c>
-      <c r="E36" t="s" s="41">
-        <v>92</v>
-      </c>
       <c r="F36" t="s" s="41">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G36" t="s" s="41">
         <v>17</v>
@@ -4048,21 +4045,21 @@
         <v>20241381</v>
       </c>
       <c r="C37" t="s" s="40">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D37" t="s" s="41">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E37" s="42">
         <v>12</v>
       </c>
       <c r="F37" t="s" s="41">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G37" s="43"/>
       <c r="H37" s="43"/>
       <c r="I37" t="s" s="41">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J37" s="44"/>
       <c r="K37" s="47"/>
@@ -4088,10 +4085,10 @@
         <v>20241385</v>
       </c>
       <c r="C38" t="s" s="40">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D38" t="s" s="41">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E38" s="42">
         <v>18000</v>
@@ -4101,7 +4098,7 @@
       <c r="H38" s="43"/>
       <c r="I38" s="43"/>
       <c r="J38" t="s" s="45">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K38" s="47"/>
       <c r="L38" s="30"/>
@@ -4126,16 +4123,16 @@
         <v>20241318</v>
       </c>
       <c r="C39" t="s" s="40">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D39" t="s" s="41">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E39" s="42">
         <v>100000</v>
       </c>
       <c r="F39" t="s" s="41">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G39" t="s" s="41">
         <v>17</v>
@@ -4166,16 +4163,16 @@
         <v>20241341</v>
       </c>
       <c r="C40" t="s" s="40">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D40" t="s" s="41">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E40" s="42">
         <v>30</v>
       </c>
       <c r="F40" t="s" s="41">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G40" t="s" s="41">
         <v>17</v>
@@ -4428,7 +4425,7 @@
       <c r="A49" s="2"/>
       <c r="B49" s="73"/>
       <c r="C49" t="s" s="74">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="9"/>
@@ -4458,7 +4455,7 @@
       <c r="A50" s="9"/>
       <c r="B50" s="77"/>
       <c r="C50" t="s" s="78">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="79"/>
@@ -4488,7 +4485,7 @@
       <c r="A51" s="9"/>
       <c r="B51" s="80"/>
       <c r="C51" t="s" s="81">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D51" s="82"/>
       <c r="E51" s="83"/>
@@ -4519,12 +4516,12 @@
       <c r="B52" s="84"/>
       <c r="C52" s="85"/>
       <c r="D52" t="s" s="86">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E52" s="87"/>
       <c r="F52" s="88"/>
       <c r="G52" t="s" s="89">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H52" s="90"/>
       <c r="I52" s="90"/>
@@ -4608,7 +4605,7 @@
       <c r="C55" s="100"/>
       <c r="D55" s="100"/>
       <c r="E55" t="s" s="101">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F55" s="102"/>
       <c r="G55" s="102"/>
@@ -4694,7 +4691,7 @@
       <c r="C58" s="114"/>
       <c r="D58" s="114"/>
       <c r="E58" t="s" s="115">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F58" s="114"/>
       <c r="G58" s="114"/>

</xml_diff>